<commit_message>
changes done in manage tag
</commit_message>
<xml_diff>
--- a/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
+++ b/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515"/>
   </bookViews>
   <sheets>
     <sheet name="Affiliate" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>testDesign4</t>
   </si>
   <si>
-    <t>testAffiliateexcel12</t>
-  </si>
-  <si>
     <t>testExcel20157813385</t>
   </si>
   <si>
@@ -95,31 +92,34 @@
     <t>testExcel23238112785454</t>
   </si>
   <si>
-    <t>testAffiliateexcel21</t>
-  </si>
-  <si>
-    <t>testAffiliateexcel33</t>
-  </si>
-  <si>
-    <t>12345647890</t>
-  </si>
-  <si>
-    <t>123456578990</t>
-  </si>
-  <si>
-    <t>123456678900</t>
-  </si>
-  <si>
-    <t>testExcel54</t>
-  </si>
-  <si>
-    <t>testExcel63</t>
-  </si>
-  <si>
-    <t>testExcel71</t>
-  </si>
-  <si>
-    <t>testExcel88</t>
+    <t>testExcel542</t>
+  </si>
+  <si>
+    <t>testExcel632</t>
+  </si>
+  <si>
+    <t>testExcel712</t>
+  </si>
+  <si>
+    <t>testExcel882</t>
+  </si>
+  <si>
+    <t>testAffiliateexcel1211</t>
+  </si>
+  <si>
+    <t>testAffiliateexcel2111</t>
+  </si>
+  <si>
+    <t>testAffiliateexcel3311</t>
+  </si>
+  <si>
+    <t>1234564783901</t>
+  </si>
+  <si>
+    <t>12345657893901</t>
+  </si>
+  <si>
+    <t>12345667893001</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,6 +171,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -491,10 +492,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -502,10 +503,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -513,10 +514,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -551,7 +552,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -559,7 +560,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -567,7 +568,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -631,41 +632,45 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>33</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="I11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created leavetype functionality and added in suite
</commit_message>
<xml_diff>
--- a/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
+++ b/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Affiliate" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="ManageTags" sheetId="3" r:id="rId3"/>
     <sheet name="Department" sheetId="4" r:id="rId4"/>
     <sheet name="Designation" sheetId="5" r:id="rId5"/>
+    <sheet name="LeaveType" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -120,6 +121,24 @@
   </si>
   <si>
     <t>12345667893001</t>
+  </si>
+  <si>
+    <t>Leave Name</t>
+  </si>
+  <si>
+    <t>Leave Abbrevation</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Casual Leave</t>
+  </si>
+  <si>
+    <t>Sick Leave</t>
+  </si>
+  <si>
+    <t>SL</t>
   </si>
 </sst>
 </file>
@@ -468,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -718,4 +737,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
created emptypes classes and its functionality added in suite
</commit_message>
<xml_diff>
--- a/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
+++ b/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Affiliate" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Department" sheetId="4" r:id="rId4"/>
     <sheet name="Designation" sheetId="5" r:id="rId5"/>
     <sheet name="LeaveType" sheetId="6" r:id="rId6"/>
+    <sheet name="EmployeeType" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -123,12 +124,6 @@
     <t>12345667893001</t>
   </si>
   <si>
-    <t>Leave Name</t>
-  </si>
-  <si>
-    <t>Leave Abbrevation</t>
-  </si>
-  <si>
     <t>CL</t>
   </si>
   <si>
@@ -139,6 +134,21 @@
   </si>
   <si>
     <t>SL</t>
+  </si>
+  <si>
+    <t>LeaveName</t>
+  </si>
+  <si>
+    <t>LeaveAbbrevation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmpCategoryName </t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
+  <si>
+    <t>Temporary</t>
   </si>
 </sst>
 </file>
@@ -743,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -754,27 +764,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes done in Branch page
</commit_message>
<xml_diff>
--- a/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
+++ b/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Affiliate" sheetId="1" r:id="rId1"/>
@@ -561,13 +561,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -796,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes done in employee page
</commit_message>
<xml_diff>
--- a/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
+++ b/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Affiliate" sheetId="1" r:id="rId1"/>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="B10:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -711,7 +711,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Created holiday and changes done in organisation pages
</commit_message>
<xml_diff>
--- a/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
+++ b/src/main/java/com/samaya/qa/testdata/Testdata.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Affiliate" sheetId="1" r:id="rId1"/>
     <sheet name="Branch" sheetId="2" r:id="rId2"/>
     <sheet name="ManageTags" sheetId="3" r:id="rId3"/>
-    <sheet name="Department" sheetId="4" r:id="rId4"/>
-    <sheet name="Designation" sheetId="5" r:id="rId5"/>
-    <sheet name="LeaveType" sheetId="6" r:id="rId6"/>
-    <sheet name="EmployeeType" sheetId="7" r:id="rId7"/>
+    <sheet name="Designation" sheetId="5" r:id="rId4"/>
+    <sheet name="LeaveType" sheetId="6" r:id="rId5"/>
+    <sheet name="Department" sheetId="7" r:id="rId6"/>
+    <sheet name="Holiday" sheetId="8" r:id="rId7"/>
+    <sheet name="EmployeeType" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -67,54 +68,9 @@
     <t>ExcelTest3</t>
   </si>
   <si>
-    <t>DeptName</t>
-  </si>
-  <si>
     <t>Designationname</t>
   </si>
   <si>
-    <t>testDesign1</t>
-  </si>
-  <si>
-    <t>testDesign2</t>
-  </si>
-  <si>
-    <t>testDesign3</t>
-  </si>
-  <si>
-    <t>testDesign4</t>
-  </si>
-  <si>
-    <t>testExcel20157813385</t>
-  </si>
-  <si>
-    <t>testExcel21311874934</t>
-  </si>
-  <si>
-    <t>testExcel23238112785454</t>
-  </si>
-  <si>
-    <t>testExcel542</t>
-  </si>
-  <si>
-    <t>testExcel632</t>
-  </si>
-  <si>
-    <t>testExcel712</t>
-  </si>
-  <si>
-    <t>testExcel882</t>
-  </si>
-  <si>
-    <t>testAffiliateexcel1211</t>
-  </si>
-  <si>
-    <t>testAffiliateexcel2111</t>
-  </si>
-  <si>
-    <t>testAffiliateexcel3311</t>
-  </si>
-  <si>
     <t>1234564783901</t>
   </si>
   <si>
@@ -127,12 +83,6 @@
     <t>CL</t>
   </si>
   <si>
-    <t>Casual Leave</t>
-  </si>
-  <si>
-    <t>Sick Leave</t>
-  </si>
-  <si>
     <t>SL</t>
   </si>
   <si>
@@ -142,13 +92,61 @@
     <t>LeaveAbbrevation</t>
   </si>
   <si>
-    <t xml:space="preserve">EmpCategoryName </t>
-  </si>
-  <si>
-    <t>Permanent</t>
-  </si>
-  <si>
-    <t>Temporary</t>
+    <t>Qa</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
+  <si>
+    <t>Sdet</t>
+  </si>
+  <si>
+    <t>DepartmentName</t>
+  </si>
+  <si>
+    <t>testAffiliateexcel1</t>
+  </si>
+  <si>
+    <t>testAffiliateexcel2</t>
+  </si>
+  <si>
+    <t>testAffiliateexcel3</t>
+  </si>
+  <si>
+    <t>testExcel1</t>
+  </si>
+  <si>
+    <t>testExcel2</t>
+  </si>
+  <si>
+    <t>testExcel3</t>
+  </si>
+  <si>
+    <t>SickLeave</t>
+  </si>
+  <si>
+    <t>CasualLeave</t>
+  </si>
+  <si>
+    <t>HolidayName</t>
+  </si>
+  <si>
+    <t>TestHoliday1</t>
+  </si>
+  <si>
+    <t>TestHoliday2</t>
+  </si>
+  <si>
+    <t>testExcel</t>
+  </si>
+  <si>
+    <t>EmpCategoryName</t>
+  </si>
+  <si>
+    <t>Temporaryusers</t>
+  </si>
+  <si>
+    <t>Permanentusers</t>
   </si>
 </sst>
 </file>
@@ -190,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -200,7 +198,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +495,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,10 +518,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -532,10 +529,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -543,10 +540,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -562,7 +559,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="B10:K23"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -581,7 +578,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -589,7 +586,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -597,7 +594,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -661,57 +658,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="I11" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -721,27 +671,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -749,12 +694,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -765,26 +710,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -792,12 +737,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -807,7 +752,83 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -817,7 +838,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>